<commit_message>
Updated formulation of grid costs
- Grid costs now accounted in Results.py file only
- Fixed error in Fixed O&M costs printing for batteries

Co-Authored-By: Gianluca Pellecchia <73592405+gianlucapellecchia@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Code/Results/Results_Summary.xlsx
+++ b/Code/Results/Results_Summary.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="75">
   <si>
     <t>Total</t>
   </si>
@@ -32,9 +32,6 @@
     <t>PV panels</t>
   </si>
   <si>
-    <t>Wind turbines</t>
-  </si>
-  <si>
     <t>Battery bank</t>
   </si>
   <si>
@@ -174,6 +171,51 @@
   </si>
   <si>
     <t>Year 5</t>
+  </si>
+  <si>
+    <t>Year 6</t>
+  </si>
+  <si>
+    <t>Year 7</t>
+  </si>
+  <si>
+    <t>Year 8</t>
+  </si>
+  <si>
+    <t>Year 9</t>
+  </si>
+  <si>
+    <t>Year 10</t>
+  </si>
+  <si>
+    <t>Year 11</t>
+  </si>
+  <si>
+    <t>Year 12</t>
+  </si>
+  <si>
+    <t>Year 13</t>
+  </si>
+  <si>
+    <t>Year 14</t>
+  </si>
+  <si>
+    <t>Year 15</t>
+  </si>
+  <si>
+    <t>Year 16</t>
+  </si>
+  <si>
+    <t>Year 17</t>
+  </si>
+  <si>
+    <t>Year 18</t>
+  </si>
+  <si>
+    <t>Year 19</t>
+  </si>
+  <si>
+    <t>Year 20</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -558,7 +600,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -580,10 +622,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2">
-        <v>81.84999999999999</v>
+        <v>57.53</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -602,21 +644,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>161.33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>9.43</v>
+        <v>22.63</v>
       </c>
     </row>
   </sheetData>
@@ -626,7 +657,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -634,13 +665,13 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -651,155 +682,155 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="E2">
-        <v>131.404</v>
+        <v>97.386</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E3">
-        <v>131.404</v>
+        <v>97.386</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="E4">
-        <v>258.82</v>
+        <v>97.02500000000001</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="E5">
-        <v>20.123</v>
+        <v>20.615</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E6">
-        <v>-20.123</v>
+        <v>-17.777</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="E7">
-        <v>-127.417</v>
+        <v>-2.478</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8">
-        <v>0.3483</v>
+        <v>0.1379</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9">
-        <v>0.3483</v>
+        <v>0.1102</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="E10">
-        <v>83.741</v>
+        <v>69.038</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -808,13 +839,13 @@
         <v>4</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="E11">
-        <v>0</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -823,253 +854,257 @@
         <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="E12">
-        <v>35.272</v>
+        <v>11.316</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="E13">
-        <v>0.886</v>
+        <v>16.67</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="B14" s="1" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="E14">
-        <v>138.92</v>
+        <v>11.755</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="E15">
-        <v>6.578</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="E16">
-        <v>0</v>
+        <v>6.021</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="E17">
-        <v>0.71</v>
+        <v>2.838</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="B18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="E18">
-        <v>0.322</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="B19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="E19">
-        <v>10.532</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>0.713</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E21">
-        <v>4.441</v>
+        <v>93.47199999999999</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C22" s="1">
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E22">
-        <v>0.024</v>
+        <v>111.962</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E23">
-        <v>23.433</v>
+        <v>4.069</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C24" s="1">
         <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E24">
-        <v>48.021</v>
+        <v>222.623</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1</v>
+        <v>35</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E25">
-        <v>0.103</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="1">
-        <v>1</v>
+        <v>36</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E26">
-        <v>34.193</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -1077,59 +1112,25 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="1">
-        <v>1</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E30">
-        <v>34.296</v>
+        <v>226.692</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1137,21 +1138,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:10">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
@@ -1159,16 +1162,13 @@
         <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1182,45 +1182,42 @@
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
@@ -1234,51 +1231,45 @@
       <c r="J3" s="1">
         <v>1</v>
       </c>
-      <c r="K3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6">
-        <v>1.74</v>
+        <v>1.38</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1287,33 +1278,30 @@
         <v>0.71</v>
       </c>
       <c r="E6">
-        <v>0.08</v>
+        <v>0.33</v>
       </c>
       <c r="F6">
-        <v>2.78</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>1.18</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>10.97</v>
       </c>
       <c r="J6">
-        <v>2.84</v>
-      </c>
-      <c r="K6">
-        <v>14.41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>13.12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7">
-        <v>1.74</v>
+        <v>1.38</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1322,33 +1310,30 @@
         <v>0.71</v>
       </c>
       <c r="E7">
-        <v>0.08</v>
+        <v>0.33</v>
       </c>
       <c r="F7">
-        <v>2.78</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>1.18</v>
+        <v>0.17</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>10.92</v>
       </c>
       <c r="J7">
-        <v>2.83</v>
-      </c>
-      <c r="K7">
-        <v>14.43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>13.06</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8">
-        <v>1.74</v>
+        <v>1.38</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1357,33 +1342,30 @@
         <v>0.71</v>
       </c>
       <c r="E8">
-        <v>0.08</v>
+        <v>0.33</v>
       </c>
       <c r="F8">
-        <v>2.78</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>1.18</v>
+        <v>0.16</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>10.93</v>
       </c>
       <c r="J8">
-        <v>2.83</v>
-      </c>
-      <c r="K8">
-        <v>14.44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>13.15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9">
-        <v>1.74</v>
+        <v>1.38</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1392,33 +1374,30 @@
         <v>0.71</v>
       </c>
       <c r="E9">
-        <v>0.08</v>
+        <v>0.33</v>
       </c>
       <c r="F9">
-        <v>2.78</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>1.16</v>
+        <v>0.04</v>
       </c>
       <c r="I9">
-        <v>0.01</v>
+        <v>10.99</v>
       </c>
       <c r="J9">
-        <v>11.19</v>
-      </c>
-      <c r="K9">
-        <v>9.960000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>13.17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10">
-        <v>1.74</v>
+        <v>1.38</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1427,30 +1406,507 @@
         <v>0.71</v>
       </c>
       <c r="E10">
+        <v>0.33</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0.06</v>
+      </c>
+      <c r="I10">
+        <v>10.99</v>
+      </c>
+      <c r="J10">
+        <v>13.12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11">
+        <v>1.38</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0.71</v>
+      </c>
+      <c r="E11">
+        <v>0.33</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="I11">
+        <v>10.98</v>
+      </c>
+      <c r="J11">
+        <v>13.19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12">
+        <v>1.38</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0.71</v>
+      </c>
+      <c r="E12">
+        <v>0.33</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
         <v>0.08</v>
       </c>
-      <c r="F10">
-        <v>2.78</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>1.16</v>
-      </c>
-      <c r="I10">
+      <c r="I12">
+        <v>10.98</v>
+      </c>
+      <c r="J12">
+        <v>13.14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13">
+        <v>1.38</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0.71</v>
+      </c>
+      <c r="E13">
+        <v>0.33</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0.11</v>
+      </c>
+      <c r="I13">
+        <v>10.96</v>
+      </c>
+      <c r="J13">
+        <v>13.16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14">
+        <v>1.38</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0.71</v>
+      </c>
+      <c r="E14">
+        <v>0.33</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0.05</v>
+      </c>
+      <c r="I14">
+        <v>11</v>
+      </c>
+      <c r="J14">
+        <v>13.12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15">
+        <v>1.38</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0.71</v>
+      </c>
+      <c r="E15">
+        <v>0.33</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0.04</v>
+      </c>
+      <c r="I15">
+        <v>11.01</v>
+      </c>
+      <c r="J15">
+        <v>13.14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16">
+        <v>1.38</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0.71</v>
+      </c>
+      <c r="E16">
+        <v>0.33</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0.08</v>
+      </c>
+      <c r="I16">
+        <v>10.99</v>
+      </c>
+      <c r="J16">
+        <v>13.17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17">
+        <v>1.38</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0.71</v>
+      </c>
+      <c r="E17">
+        <v>0.33</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0.06</v>
+      </c>
+      <c r="I17">
+        <v>11</v>
+      </c>
+      <c r="J17">
+        <v>13.16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18">
+        <v>1.38</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0.71</v>
+      </c>
+      <c r="E18">
+        <v>0.33</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="I18">
+        <v>11</v>
+      </c>
+      <c r="J18">
+        <v>13.19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19">
+        <v>1.38</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0.71</v>
+      </c>
+      <c r="E19">
+        <v>0.33</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0.13</v>
+      </c>
+      <c r="I19">
+        <v>10.97</v>
+      </c>
+      <c r="J19">
+        <v>13.16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20">
+        <v>1.38</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0.71</v>
+      </c>
+      <c r="E20">
+        <v>0.33</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0.06</v>
+      </c>
+      <c r="I20">
+        <v>11.02</v>
+      </c>
+      <c r="J20">
+        <v>13.21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21">
+        <v>1.38</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0.71</v>
+      </c>
+      <c r="E21">
+        <v>0.33</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0.03</v>
+      </c>
+      <c r="I21">
+        <v>11.04</v>
+      </c>
+      <c r="J21">
+        <v>13.23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22">
+        <v>1.38</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0.71</v>
+      </c>
+      <c r="E22">
+        <v>0.33</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
         <v>0.02</v>
       </c>
-      <c r="J10">
-        <v>14.08</v>
-      </c>
-      <c r="K10">
-        <v>8.609999999999999</v>
+      <c r="I22">
+        <v>11.05</v>
+      </c>
+      <c r="J22">
+        <v>13.22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23">
+        <v>1.38</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0.71</v>
+      </c>
+      <c r="E23">
+        <v>0.33</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0.09</v>
+      </c>
+      <c r="I23">
+        <v>11.02</v>
+      </c>
+      <c r="J23">
+        <v>13.18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24">
+        <v>1.38</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0.71</v>
+      </c>
+      <c r="E24">
+        <v>0.33</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="I24">
+        <v>11.03</v>
+      </c>
+      <c r="J24">
+        <v>13.26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25">
+        <v>1.38</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0.71</v>
+      </c>
+      <c r="E25">
+        <v>0.33</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0.06</v>
+      </c>
+      <c r="I25">
+        <v>11.04</v>
+      </c>
+      <c r="J25">
+        <v>13.24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1458,7 +1914,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1467,139 +1923,439 @@
     <row r="1" spans="1:6">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>0.19</v>
       </c>
       <c r="C4">
-        <v>91.73</v>
+        <v>66.76000000000001</v>
       </c>
       <c r="D4">
-        <v>0.09</v>
+        <v>0.35</v>
       </c>
       <c r="E4">
-        <v>34.85</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>15.12</v>
+        <v>55.1</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5">
-        <v>0.01</v>
+        <v>0.47</v>
       </c>
       <c r="C5">
-        <v>91.73999999999999</v>
+        <v>66.75</v>
       </c>
       <c r="D5">
-        <v>0.02</v>
+        <v>0.64</v>
       </c>
       <c r="E5">
-        <v>34.83</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>15.11</v>
+        <v>54.82</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>0.44</v>
       </c>
       <c r="C6">
-        <v>91.75</v>
+        <v>66.75</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>0.26</v>
       </c>
       <c r="E6">
-        <v>34.85</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>15.09</v>
+        <v>54.87</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7">
-        <v>0.03</v>
+        <v>0.12</v>
       </c>
       <c r="C7">
-        <v>73.76000000000001</v>
+        <v>66.75</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="E7">
-        <v>20.38</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>35.37</v>
+        <v>55.2</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8">
+        <v>0.16</v>
+      </c>
+      <c r="C8">
+        <v>66.73999999999999</v>
+      </c>
+      <c r="D8">
+        <v>0.39</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>55.17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B8">
-        <v>0.04</v>
-      </c>
-      <c r="C8">
-        <v>69.08</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>17.86</v>
-      </c>
-      <c r="F8">
-        <v>39.24</v>
+      <c r="B9">
+        <v>0.21</v>
+      </c>
+      <c r="C9">
+        <v>66.73999999999999</v>
+      </c>
+      <c r="D9">
+        <v>0.09</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>55.13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10">
+        <v>0.22</v>
+      </c>
+      <c r="C10">
+        <v>66.73</v>
+      </c>
+      <c r="D10">
+        <v>0.31</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>55.13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11">
+        <v>0.32</v>
+      </c>
+      <c r="C11">
+        <v>66.73</v>
+      </c>
+      <c r="D11">
+        <v>0.26</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>55.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12">
+        <v>0.14</v>
+      </c>
+      <c r="C12">
+        <v>66.72</v>
+      </c>
+      <c r="D12">
+        <v>0.44</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>55.24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13">
+        <v>0.11</v>
+      </c>
+      <c r="C13">
+        <v>66.72</v>
+      </c>
+      <c r="D13">
+        <v>0.38</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>55.28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14">
+        <v>0.24</v>
+      </c>
+      <c r="C14">
+        <v>66.70999999999999</v>
+      </c>
+      <c r="D14">
+        <v>0.23</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>55.17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15">
+        <v>0.17</v>
+      </c>
+      <c r="C15">
+        <v>66.7</v>
+      </c>
+      <c r="D15">
+        <v>0.29</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>55.26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16">
+        <v>0.2</v>
+      </c>
+      <c r="C16">
+        <v>66.69</v>
+      </c>
+      <c r="D16">
+        <v>0.17</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>55.24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17">
+        <v>0.37</v>
+      </c>
+      <c r="C17">
+        <v>66.69</v>
+      </c>
+      <c r="D17">
+        <v>0.35</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>55.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18">
+        <v>0.17</v>
+      </c>
+      <c r="C18">
+        <v>66.68000000000001</v>
+      </c>
+      <c r="D18">
+        <v>0.14</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>55.32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19">
+        <v>0.09</v>
+      </c>
+      <c r="C19">
+        <v>66.67</v>
+      </c>
+      <c r="D19">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>55.43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20">
+        <v>0.06</v>
+      </c>
+      <c r="C20">
+        <v>66.65000000000001</v>
+      </c>
+      <c r="D20">
+        <v>0.13</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>55.48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21">
+        <v>0.24</v>
+      </c>
+      <c r="C21">
+        <v>66.64</v>
+      </c>
+      <c r="D21">
+        <v>0.33</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>55.33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22">
+        <v>0.2</v>
+      </c>
+      <c r="C22">
+        <v>66.63</v>
+      </c>
+      <c r="D22">
+        <v>0.03</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>55.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23">
+        <v>0.18</v>
+      </c>
+      <c r="C23">
+        <v>66.62</v>
+      </c>
+      <c r="D23">
+        <v>0.14</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>55.46</v>
       </c>
     </row>
   </sheetData>
@@ -1609,57 +2365,53 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="E1" s="1" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -1676,152 +2428,428 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6">
+        <v>0.19</v>
+      </c>
+      <c r="C6">
+        <v>66.76000000000001</v>
+      </c>
+      <c r="D6">
+        <v>0.35</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>55.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7">
+        <v>0.47</v>
+      </c>
+      <c r="C7">
+        <v>66.75</v>
+      </c>
+      <c r="D7">
+        <v>0.64</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>54.82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8">
+        <v>0.44</v>
+      </c>
+      <c r="C8">
+        <v>66.75</v>
+      </c>
+      <c r="D8">
+        <v>0.26</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>54.87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9">
+        <v>0.12</v>
+      </c>
+      <c r="C9">
+        <v>66.75</v>
+      </c>
+      <c r="D9">
+        <v>0.14</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>55.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10">
+        <v>0.16</v>
+      </c>
+      <c r="C10">
+        <v>66.73999999999999</v>
+      </c>
+      <c r="D10">
+        <v>0.39</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>55.17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11">
+        <v>0.21</v>
+      </c>
+      <c r="C11">
+        <v>66.73999999999999</v>
+      </c>
+      <c r="D11">
+        <v>0.09</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>55.13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B12">
+        <v>0.22</v>
+      </c>
+      <c r="C12">
+        <v>66.73</v>
+      </c>
+      <c r="D12">
+        <v>0.31</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>55.13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13">
+        <v>0.32</v>
+      </c>
+      <c r="C13">
+        <v>66.73</v>
+      </c>
+      <c r="D13">
+        <v>0.26</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>55.05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14">
+        <v>0.14</v>
+      </c>
+      <c r="C14">
+        <v>66.72</v>
+      </c>
+      <c r="D14">
+        <v>0.44</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>55.24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15">
+        <v>0.11</v>
+      </c>
+      <c r="C15">
+        <v>66.72</v>
+      </c>
+      <c r="D15">
+        <v>0.38</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>55.28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16">
+        <v>0.24</v>
+      </c>
+      <c r="C16">
+        <v>66.70999999999999</v>
+      </c>
+      <c r="D16">
+        <v>0.23</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>55.17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17">
+        <v>0.17</v>
+      </c>
+      <c r="C17">
+        <v>66.7</v>
+      </c>
+      <c r="D17">
+        <v>0.29</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>55.26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>91.73</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
+      <c r="B18">
+        <v>0.2</v>
+      </c>
+      <c r="C18">
+        <v>66.69</v>
+      </c>
+      <c r="D18">
+        <v>0.17</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>55.24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19">
+        <v>0.37</v>
+      </c>
+      <c r="C19">
+        <v>66.69</v>
+      </c>
+      <c r="D19">
+        <v>0.35</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>55.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20">
+        <v>0.17</v>
+      </c>
+      <c r="C20">
+        <v>66.68000000000001</v>
+      </c>
+      <c r="D20">
+        <v>0.14</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>55.32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21">
         <v>0.09</v>
       </c>
-      <c r="F6">
-        <v>34.85</v>
-      </c>
-      <c r="G6">
-        <v>15.12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7">
-        <v>0.01</v>
-      </c>
-      <c r="C7">
-        <v>91.73999999999999</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0.02</v>
-      </c>
-      <c r="F7">
-        <v>34.83</v>
-      </c>
-      <c r="G7">
-        <v>15.11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>91.75</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>34.85</v>
-      </c>
-      <c r="G8">
-        <v>15.09</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9">
+      <c r="C21">
+        <v>66.67</v>
+      </c>
+      <c r="D21">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>55.43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22">
+        <v>0.06</v>
+      </c>
+      <c r="C22">
+        <v>66.65000000000001</v>
+      </c>
+      <c r="D22">
+        <v>0.13</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>55.48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23">
+        <v>0.24</v>
+      </c>
+      <c r="C23">
+        <v>66.64</v>
+      </c>
+      <c r="D23">
+        <v>0.33</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>55.33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24">
+        <v>0.2</v>
+      </c>
+      <c r="C24">
+        <v>66.63</v>
+      </c>
+      <c r="D24">
         <v>0.03</v>
       </c>
-      <c r="C9">
-        <v>73.76000000000001</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>20.38</v>
-      </c>
-      <c r="G9">
-        <v>35.37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10">
-        <v>0.04</v>
-      </c>
-      <c r="C10">
-        <v>69.08</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>17.86</v>
-      </c>
-      <c r="G10">
-        <v>39.24</v>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>55.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25">
+        <v>0.18</v>
+      </c>
+      <c r="C25">
+        <v>66.62</v>
+      </c>
+      <c r="D25">
+        <v>0.14</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>55.46</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C1:D1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change in solver options
</commit_message>
<xml_diff>
--- a/Code/Results/Results_Summary.xlsx
+++ b/Code/Results/Results_Summary.xlsx
@@ -448,7 +448,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>156.94</v>
+        <v>131.13</v>
       </c>
     </row>
     <row r="3">
@@ -463,7 +463,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>436.17</v>
+        <v>529.75</v>
       </c>
     </row>
     <row r="4">
@@ -478,7 +478,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>24.68</v>
+        <v>32.32</v>
       </c>
     </row>
   </sheetData>
@@ -549,7 +549,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>856.13</v>
+        <v>376.18</v>
       </c>
     </row>
     <row r="3">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>856.13</v>
+        <v>376.18</v>
       </c>
     </row>
     <row r="4">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>887.96</v>
+        <v>147.969</v>
       </c>
     </row>
     <row r="5">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>165.155</v>
+        <v>47.479</v>
       </c>
     </row>
     <row r="6">
@@ -645,7 +645,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>-47.031</v>
+        <v>184.297</v>
       </c>
     </row>
     <row r="7">
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>-149.954</v>
+        <v>-3.565</v>
       </c>
     </row>
     <row r="8">
@@ -695,7 +695,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>0.4666</v>
+        <v>0.205</v>
       </c>
     </row>
     <row r="9">
@@ -718,7 +718,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0.0009</v>
+        <v>0.205</v>
       </c>
     </row>
     <row r="10">
@@ -743,7 +743,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>134.557</v>
+        <v>107.199</v>
       </c>
     </row>
     <row r="11">
@@ -764,7 +764,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>7.254</v>
+        <v>27.841</v>
       </c>
     </row>
     <row r="12">
@@ -785,7 +785,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>9.872999999999999</v>
+        <v>12.928</v>
       </c>
     </row>
     <row r="13">
@@ -806,7 +806,7 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>736.276</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -831,7 +831,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>26.689</v>
+        <v>22.3</v>
       </c>
     </row>
     <row r="15">
@@ -852,7 +852,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>15.395</v>
+        <v>18.697</v>
       </c>
     </row>
     <row r="16">
@@ -873,7 +873,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>4.95</v>
+        <v>6.482</v>
       </c>
     </row>
     <row r="17">
@@ -894,7 +894,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>118.122</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -940,7 +940,7 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>24.666</v>
+        <v>27.883</v>
       </c>
     </row>
     <row r="20">
@@ -963,7 +963,7 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>0.158</v>
+        <v>156.414</v>
       </c>
     </row>
     <row r="21">
@@ -986,7 +986,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>88.797</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1009,7 +1009,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>160.652</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>1.262</v>
+        <v>1060.636</v>
       </c>
     </row>
     <row r="24">
@@ -1055,7 +1055,7 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>76.322</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1153,7 +1153,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>77.584</v>
+        <v>1060.636</v>
       </c>
     </row>
   </sheetData>
@@ -1368,31 +1368,31 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3.33</v>
+        <v>2.78</v>
       </c>
       <c r="C6" t="n">
-        <v>1.92</v>
+        <v>2.33</v>
       </c>
       <c r="D6" t="n">
-        <v>0.62</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E6" t="n">
-        <v>14.73</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>2.94</v>
+        <v>3.07</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>0.52</v>
       </c>
       <c r="I6" t="n">
-        <v>0.67</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>30.07</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -1402,31 +1402,31 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3.33</v>
+        <v>2.78</v>
       </c>
       <c r="C7" t="n">
-        <v>1.92</v>
+        <v>2.33</v>
       </c>
       <c r="D7" t="n">
-        <v>0.62</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E7" t="n">
-        <v>14.73</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>3.14</v>
+        <v>3.41</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>1.39</v>
       </c>
       <c r="I7" t="n">
-        <v>1.78</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>27.27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -1436,31 +1436,31 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>3.33</v>
+        <v>2.78</v>
       </c>
       <c r="C8" t="n">
-        <v>1.92</v>
+        <v>2.33</v>
       </c>
       <c r="D8" t="n">
-        <v>0.62</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E8" t="n">
-        <v>14.73</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>3.15</v>
+        <v>3.49</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>1.78</v>
       </c>
       <c r="I8" t="n">
-        <v>2.27</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1470,31 +1470,31 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3.33</v>
+        <v>2.78</v>
       </c>
       <c r="C9" t="n">
-        <v>1.92</v>
+        <v>2.33</v>
       </c>
       <c r="D9" t="n">
-        <v>0.62</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E9" t="n">
-        <v>14.73</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>3.14</v>
+        <v>3.69</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>4.22</v>
       </c>
       <c r="I9" t="n">
-        <v>4.53</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>25.31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -1504,31 +1504,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3.33</v>
+        <v>2.78</v>
       </c>
       <c r="C10" t="n">
-        <v>1.92</v>
+        <v>2.33</v>
       </c>
       <c r="D10" t="n">
-        <v>0.62</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E10" t="n">
-        <v>14.73</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>3.12</v>
+        <v>3.66</v>
       </c>
       <c r="H10" t="n">
-        <v>0.02</v>
+        <v>13.87</v>
       </c>
       <c r="I10" t="n">
-        <v>9.210000000000001</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
-        <v>20.49</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -1538,31 +1538,31 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>3.33</v>
+        <v>2.78</v>
       </c>
       <c r="C11" t="n">
-        <v>1.92</v>
+        <v>2.33</v>
       </c>
       <c r="D11" t="n">
-        <v>0.62</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E11" t="n">
-        <v>14.73</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>3.11</v>
+        <v>3.64</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>15.21</v>
       </c>
       <c r="I11" t="n">
-        <v>9.81</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>19.52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1572,31 +1572,31 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>3.33</v>
+        <v>2.78</v>
       </c>
       <c r="C12" t="n">
-        <v>1.92</v>
+        <v>2.33</v>
       </c>
       <c r="D12" t="n">
-        <v>0.62</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E12" t="n">
-        <v>14.73</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>3.09</v>
+        <v>3.59</v>
       </c>
       <c r="H12" t="n">
-        <v>0.01</v>
+        <v>28.04</v>
       </c>
       <c r="I12" t="n">
-        <v>15.95</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>16.46</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1606,31 +1606,31 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>3.33</v>
+        <v>2.78</v>
       </c>
       <c r="C13" t="n">
-        <v>1.92</v>
+        <v>2.33</v>
       </c>
       <c r="D13" t="n">
-        <v>0.62</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E13" t="n">
-        <v>14.73</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>3.09</v>
+        <v>3.59</v>
       </c>
       <c r="H13" t="n">
-        <v>0.09</v>
+        <v>28.26</v>
       </c>
       <c r="I13" t="n">
-        <v>15.99</v>
+        <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>16.47</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1640,31 +1640,31 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>3.33</v>
+        <v>2.78</v>
       </c>
       <c r="C14" t="n">
-        <v>1.92</v>
+        <v>2.33</v>
       </c>
       <c r="D14" t="n">
-        <v>0.62</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E14" t="n">
-        <v>14.73</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>3.08</v>
+        <v>3.58</v>
       </c>
       <c r="H14" t="n">
-        <v>0.01</v>
+        <v>29.76</v>
       </c>
       <c r="I14" t="n">
-        <v>16.72</v>
+        <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>15.92</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -1674,31 +1674,31 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>3.33</v>
+        <v>2.78</v>
       </c>
       <c r="C15" t="n">
-        <v>1.92</v>
+        <v>2.33</v>
       </c>
       <c r="D15" t="n">
-        <v>0.62</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E15" t="n">
-        <v>14.73</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>3.08</v>
+        <v>3.58</v>
       </c>
       <c r="H15" t="n">
-        <v>0.05</v>
+        <v>30.35</v>
       </c>
       <c r="I15" t="n">
-        <v>16.98</v>
+        <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>15.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -1708,31 +1708,31 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>3.33</v>
+        <v>2.78</v>
       </c>
       <c r="C16" t="n">
-        <v>1.92</v>
+        <v>2.33</v>
       </c>
       <c r="D16" t="n">
-        <v>0.62</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E16" t="n">
-        <v>14.73</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>3.04</v>
+        <v>3.43</v>
       </c>
       <c r="H16" t="n">
-        <v>0.07000000000000001</v>
+        <v>37.98</v>
       </c>
       <c r="I16" t="n">
-        <v>19.9</v>
+        <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>12.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1742,31 +1742,31 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>3.33</v>
+        <v>2.78</v>
       </c>
       <c r="C17" t="n">
-        <v>1.92</v>
+        <v>2.33</v>
       </c>
       <c r="D17" t="n">
-        <v>0.62</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E17" t="n">
-        <v>14.73</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>3.03</v>
+        <v>3.43</v>
       </c>
       <c r="H17" t="n">
-        <v>0.07000000000000001</v>
+        <v>38.14</v>
       </c>
       <c r="I17" t="n">
-        <v>19.96</v>
+        <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>12.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1776,31 +1776,31 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>3.33</v>
+        <v>2.78</v>
       </c>
       <c r="C18" t="n">
-        <v>1.92</v>
+        <v>2.33</v>
       </c>
       <c r="D18" t="n">
-        <v>0.62</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E18" t="n">
-        <v>14.73</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>3.03</v>
+        <v>3.44</v>
       </c>
       <c r="H18" t="n">
-        <v>0.04</v>
+        <v>41.93</v>
       </c>
       <c r="I18" t="n">
-        <v>21.52</v>
+        <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>11.24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1810,31 +1810,31 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>3.33</v>
+        <v>2.78</v>
       </c>
       <c r="C19" t="n">
-        <v>1.92</v>
+        <v>2.33</v>
       </c>
       <c r="D19" t="n">
-        <v>0.62</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E19" t="n">
-        <v>14.73</v>
+        <v>0</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>3.02</v>
+        <v>3.39</v>
       </c>
       <c r="H19" t="n">
-        <v>0.01</v>
+        <v>45.83</v>
       </c>
       <c r="I19" t="n">
-        <v>23.01</v>
+        <v>0</v>
       </c>
       <c r="J19" t="n">
-        <v>10.38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1844,31 +1844,31 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>3.33</v>
+        <v>2.78</v>
       </c>
       <c r="C20" t="n">
-        <v>1.92</v>
+        <v>2.33</v>
       </c>
       <c r="D20" t="n">
-        <v>0.62</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E20" t="n">
-        <v>14.73</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>3.01</v>
+        <v>3.37</v>
       </c>
       <c r="H20" t="n">
-        <v>0.05</v>
+        <v>48.58</v>
       </c>
       <c r="I20" t="n">
-        <v>24.02</v>
+        <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>9.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1878,31 +1878,31 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>3.33</v>
+        <v>2.78</v>
       </c>
       <c r="C21" t="n">
-        <v>1.92</v>
+        <v>2.33</v>
       </c>
       <c r="D21" t="n">
-        <v>0.62</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E21" t="n">
-        <v>14.73</v>
+        <v>0</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>3.01</v>
+        <v>3.37</v>
       </c>
       <c r="H21" t="n">
-        <v>0</v>
+        <v>48.57</v>
       </c>
       <c r="I21" t="n">
-        <v>24.06</v>
+        <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>9.83</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1912,31 +1912,31 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>3.33</v>
+        <v>2.78</v>
       </c>
       <c r="C22" t="n">
-        <v>1.92</v>
+        <v>2.33</v>
       </c>
       <c r="D22" t="n">
-        <v>0.62</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E22" t="n">
-        <v>14.73</v>
+        <v>0</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>3.01</v>
+        <v>3.36</v>
       </c>
       <c r="H22" t="n">
-        <v>0.03</v>
+        <v>48.56</v>
       </c>
       <c r="I22" t="n">
-        <v>24.04</v>
+        <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>9.82</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2028,19 +2028,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="C4" t="n">
-        <v>98.88</v>
+        <v>99.47</v>
       </c>
       <c r="D4" t="n">
-        <v>0.13</v>
+        <v>39.93</v>
       </c>
       <c r="E4" t="n">
-        <v>51.67</v>
+        <v>53.83</v>
       </c>
       <c r="F4" t="n">
-        <v>2.44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -2050,19 +2050,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>2.26</v>
       </c>
       <c r="C5" t="n">
-        <v>97.09999999999999</v>
+        <v>98.59</v>
       </c>
       <c r="D5" t="n">
-        <v>0.15</v>
+        <v>32.47</v>
       </c>
       <c r="E5" t="n">
-        <v>48.5</v>
+        <v>52.77</v>
       </c>
       <c r="F5" t="n">
-        <v>5.66</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -2072,19 +2072,19 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>2.83</v>
       </c>
       <c r="C6" t="n">
-        <v>96.33</v>
+        <v>98.2</v>
       </c>
       <c r="D6" t="n">
-        <v>0.12</v>
+        <v>31.1</v>
       </c>
       <c r="E6" t="n">
-        <v>47.5</v>
+        <v>52.58</v>
       </c>
       <c r="F6" t="n">
-        <v>7.06</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -2094,19 +2094,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>5.98</v>
       </c>
       <c r="C7" t="n">
-        <v>92.94</v>
+        <v>95.84999999999999</v>
       </c>
       <c r="D7" t="n">
-        <v>0.32</v>
+        <v>25.03</v>
       </c>
       <c r="E7" t="n">
-        <v>42.37</v>
+        <v>49.78</v>
       </c>
       <c r="F7" t="n">
-        <v>12.58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -2116,19 +2116,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.02</v>
+        <v>15.5</v>
       </c>
       <c r="C8" t="n">
-        <v>86.59999999999999</v>
+        <v>87.54000000000001</v>
       </c>
       <c r="D8" t="n">
-        <v>0.09</v>
+        <v>14.54</v>
       </c>
       <c r="E8" t="n">
-        <v>33.09</v>
+        <v>38.81</v>
       </c>
       <c r="F8" t="n">
-        <v>20.16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -2138,19 +2138,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>16.46</v>
       </c>
       <c r="C9" t="n">
-        <v>85.86</v>
+        <v>86.5</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2</v>
+        <v>12.98</v>
       </c>
       <c r="E9" t="n">
-        <v>31.99</v>
+        <v>37.43</v>
       </c>
       <c r="F9" t="n">
-        <v>20.79</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -2160,19 +2160,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.02</v>
+        <v>25.39</v>
       </c>
       <c r="C10" t="n">
-        <v>78.88</v>
+        <v>77.66</v>
       </c>
       <c r="D10" t="n">
-        <v>0.24</v>
+        <v>7.57</v>
       </c>
       <c r="E10" t="n">
-        <v>26.54</v>
+        <v>30.89</v>
       </c>
       <c r="F10" t="n">
-        <v>28.27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -2182,19 +2182,19 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.1</v>
+        <v>25.51</v>
       </c>
       <c r="C11" t="n">
-        <v>78.78</v>
+        <v>77.52</v>
       </c>
       <c r="D11" t="n">
-        <v>0.06</v>
+        <v>7.44</v>
       </c>
       <c r="E11" t="n">
-        <v>26.45</v>
+        <v>30.78</v>
       </c>
       <c r="F11" t="n">
-        <v>28.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -2204,19 +2204,19 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.01</v>
+        <v>26.29</v>
       </c>
       <c r="C12" t="n">
-        <v>78.09</v>
+        <v>76.61</v>
       </c>
       <c r="D12" t="n">
-        <v>0.09</v>
+        <v>6.66</v>
       </c>
       <c r="E12" t="n">
-        <v>25.82</v>
+        <v>30.02</v>
       </c>
       <c r="F12" t="n">
-        <v>28.91</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -2226,19 +2226,19 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.05</v>
+        <v>26.66</v>
       </c>
       <c r="C13" t="n">
-        <v>77.79000000000001</v>
+        <v>76.25</v>
       </c>
       <c r="D13" t="n">
-        <v>0.25</v>
+        <v>6.59</v>
       </c>
       <c r="E13" t="n">
-        <v>25.69</v>
+        <v>29.85</v>
       </c>
       <c r="F13" t="n">
-        <v>29.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -2248,19 +2248,19 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.07000000000000001</v>
+        <v>29.89</v>
       </c>
       <c r="C14" t="n">
-        <v>74.92</v>
+        <v>71.95999999999999</v>
       </c>
       <c r="D14" t="n">
-        <v>0.11</v>
+        <v>2.25</v>
       </c>
       <c r="E14" t="n">
-        <v>22.7</v>
+        <v>25.68</v>
       </c>
       <c r="F14" t="n">
-        <v>30.66</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -2270,19 +2270,19 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.06</v>
+        <v>29.99</v>
       </c>
       <c r="C15" t="n">
-        <v>74.87</v>
+        <v>71.87</v>
       </c>
       <c r="D15" t="n">
-        <v>0.08</v>
+        <v>2.27</v>
       </c>
       <c r="E15" t="n">
-        <v>22.65</v>
+        <v>25.64</v>
       </c>
       <c r="F15" t="n">
-        <v>30.72</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -2292,19 +2292,19 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.04</v>
+        <v>31.79</v>
       </c>
       <c r="C16" t="n">
-        <v>73.45</v>
+        <v>69.92</v>
       </c>
       <c r="D16" t="n">
-        <v>0.09</v>
+        <v>1.54</v>
       </c>
       <c r="E16" t="n">
-        <v>21.84</v>
+        <v>24.81</v>
       </c>
       <c r="F16" t="n">
-        <v>31.94</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -2314,19 +2314,19 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.01</v>
+        <v>33.56</v>
       </c>
       <c r="C17" t="n">
-        <v>72.14</v>
+        <v>68.01000000000001</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>1.02</v>
       </c>
       <c r="E17" t="n">
-        <v>21</v>
+        <v>23.6</v>
       </c>
       <c r="F17" t="n">
-        <v>32.97</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -2336,19 +2336,19 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.05</v>
+        <v>34.76</v>
       </c>
       <c r="C18" t="n">
-        <v>71.25</v>
+        <v>66.73</v>
       </c>
       <c r="D18" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.71</v>
       </c>
       <c r="E18" t="n">
-        <v>20.48</v>
+        <v>22.88</v>
       </c>
       <c r="F18" t="n">
-        <v>33.63</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -2358,19 +2358,19 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>34.76</v>
       </c>
       <c r="C19" t="n">
-        <v>71.23999999999999</v>
+        <v>66.73999999999999</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>0.74</v>
       </c>
       <c r="E19" t="n">
-        <v>20.47</v>
+        <v>22.88</v>
       </c>
       <c r="F19" t="n">
-        <v>33.71</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -2380,19 +2380,19 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.02</v>
+        <v>34.75</v>
       </c>
       <c r="C20" t="n">
-        <v>71.23999999999999</v>
+        <v>66.73999999999999</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>0.73</v>
       </c>
       <c r="E20" t="n">
-        <v>20.46</v>
+        <v>22.85</v>
       </c>
       <c r="F20" t="n">
-        <v>33.67</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2535,19 +2535,19 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="C6" t="n">
-        <v>98.88</v>
+        <v>99.47</v>
       </c>
       <c r="D6" t="n">
-        <v>0.13</v>
+        <v>39.93</v>
       </c>
       <c r="E6" t="n">
-        <v>51.67</v>
+        <v>53.83</v>
       </c>
       <c r="F6" t="n">
-        <v>2.44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -2557,19 +2557,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>2.26</v>
       </c>
       <c r="C7" t="n">
-        <v>97.09999999999999</v>
+        <v>98.59</v>
       </c>
       <c r="D7" t="n">
-        <v>0.15</v>
+        <v>32.47</v>
       </c>
       <c r="E7" t="n">
-        <v>48.5</v>
+        <v>52.77</v>
       </c>
       <c r="F7" t="n">
-        <v>5.66</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -2579,19 +2579,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>2.83</v>
       </c>
       <c r="C8" t="n">
-        <v>96.33</v>
+        <v>98.2</v>
       </c>
       <c r="D8" t="n">
-        <v>0.12</v>
+        <v>31.1</v>
       </c>
       <c r="E8" t="n">
-        <v>47.5</v>
+        <v>52.58</v>
       </c>
       <c r="F8" t="n">
-        <v>7.06</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -2601,19 +2601,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>5.98</v>
       </c>
       <c r="C9" t="n">
-        <v>92.94</v>
+        <v>95.84999999999999</v>
       </c>
       <c r="D9" t="n">
-        <v>0.32</v>
+        <v>25.03</v>
       </c>
       <c r="E9" t="n">
-        <v>42.37</v>
+        <v>49.78</v>
       </c>
       <c r="F9" t="n">
-        <v>12.58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -2623,19 +2623,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.02</v>
+        <v>15.5</v>
       </c>
       <c r="C10" t="n">
-        <v>86.59999999999999</v>
+        <v>87.54000000000001</v>
       </c>
       <c r="D10" t="n">
-        <v>0.09</v>
+        <v>14.54</v>
       </c>
       <c r="E10" t="n">
-        <v>33.09</v>
+        <v>38.81</v>
       </c>
       <c r="F10" t="n">
-        <v>20.16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -2645,19 +2645,19 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>16.46</v>
       </c>
       <c r="C11" t="n">
-        <v>85.86</v>
+        <v>86.5</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2</v>
+        <v>12.98</v>
       </c>
       <c r="E11" t="n">
-        <v>31.99</v>
+        <v>37.43</v>
       </c>
       <c r="F11" t="n">
-        <v>20.79</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -2667,19 +2667,19 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.02</v>
+        <v>25.39</v>
       </c>
       <c r="C12" t="n">
-        <v>78.88</v>
+        <v>77.66</v>
       </c>
       <c r="D12" t="n">
-        <v>0.24</v>
+        <v>7.57</v>
       </c>
       <c r="E12" t="n">
-        <v>26.54</v>
+        <v>30.89</v>
       </c>
       <c r="F12" t="n">
-        <v>28.27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -2689,19 +2689,19 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.1</v>
+        <v>25.51</v>
       </c>
       <c r="C13" t="n">
-        <v>78.78</v>
+        <v>77.52</v>
       </c>
       <c r="D13" t="n">
-        <v>0.06</v>
+        <v>7.44</v>
       </c>
       <c r="E13" t="n">
-        <v>26.45</v>
+        <v>30.78</v>
       </c>
       <c r="F13" t="n">
-        <v>28.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -2711,19 +2711,19 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.01</v>
+        <v>26.29</v>
       </c>
       <c r="C14" t="n">
-        <v>78.09</v>
+        <v>76.61</v>
       </c>
       <c r="D14" t="n">
-        <v>0.09</v>
+        <v>6.66</v>
       </c>
       <c r="E14" t="n">
-        <v>25.82</v>
+        <v>30.02</v>
       </c>
       <c r="F14" t="n">
-        <v>28.91</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -2733,19 +2733,19 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.05</v>
+        <v>26.66</v>
       </c>
       <c r="C15" t="n">
-        <v>77.79000000000001</v>
+        <v>76.25</v>
       </c>
       <c r="D15" t="n">
-        <v>0.25</v>
+        <v>6.59</v>
       </c>
       <c r="E15" t="n">
-        <v>25.69</v>
+        <v>29.85</v>
       </c>
       <c r="F15" t="n">
-        <v>29.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -2755,19 +2755,19 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.07000000000000001</v>
+        <v>29.89</v>
       </c>
       <c r="C16" t="n">
-        <v>74.92</v>
+        <v>71.95999999999999</v>
       </c>
       <c r="D16" t="n">
-        <v>0.11</v>
+        <v>2.25</v>
       </c>
       <c r="E16" t="n">
-        <v>22.7</v>
+        <v>25.68</v>
       </c>
       <c r="F16" t="n">
-        <v>30.66</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -2777,19 +2777,19 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.06</v>
+        <v>29.99</v>
       </c>
       <c r="C17" t="n">
-        <v>74.87</v>
+        <v>71.87</v>
       </c>
       <c r="D17" t="n">
-        <v>0.08</v>
+        <v>2.27</v>
       </c>
       <c r="E17" t="n">
-        <v>22.65</v>
+        <v>25.64</v>
       </c>
       <c r="F17" t="n">
-        <v>30.72</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -2799,19 +2799,19 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.04</v>
+        <v>31.79</v>
       </c>
       <c r="C18" t="n">
-        <v>73.45</v>
+        <v>69.92</v>
       </c>
       <c r="D18" t="n">
-        <v>0.09</v>
+        <v>1.54</v>
       </c>
       <c r="E18" t="n">
-        <v>21.84</v>
+        <v>24.81</v>
       </c>
       <c r="F18" t="n">
-        <v>31.94</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -2821,19 +2821,19 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.01</v>
+        <v>33.56</v>
       </c>
       <c r="C19" t="n">
-        <v>72.14</v>
+        <v>68.01000000000001</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>1.02</v>
       </c>
       <c r="E19" t="n">
-        <v>21</v>
+        <v>23.6</v>
       </c>
       <c r="F19" t="n">
-        <v>32.97</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -2843,19 +2843,19 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.05</v>
+        <v>34.76</v>
       </c>
       <c r="C20" t="n">
-        <v>71.25</v>
+        <v>66.73</v>
       </c>
       <c r="D20" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.71</v>
       </c>
       <c r="E20" t="n">
-        <v>20.48</v>
+        <v>22.88</v>
       </c>
       <c r="F20" t="n">
-        <v>33.63</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -2865,19 +2865,19 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0</v>
+        <v>34.76</v>
       </c>
       <c r="C21" t="n">
-        <v>71.23999999999999</v>
+        <v>66.73999999999999</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>0.74</v>
       </c>
       <c r="E21" t="n">
-        <v>20.47</v>
+        <v>22.88</v>
       </c>
       <c r="F21" t="n">
-        <v>33.71</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -2887,19 +2887,19 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.02</v>
+        <v>34.75</v>
       </c>
       <c r="C22" t="n">
-        <v>71.23999999999999</v>
+        <v>66.73999999999999</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>0.73</v>
       </c>
       <c r="E22" t="n">
-        <v>20.46</v>
+        <v>22.85</v>
       </c>
       <c r="F22" t="n">
-        <v>33.67</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>